<commit_message>
RQ - ST tracciamento xlsx completo
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Specifica Tecnica/Tracciamento Classi-requisiti.xlsx
+++ b/RQ/Esterni/Specifica Tecnica/Tracciamento Classi-requisiti.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="152">
   <si>
     <t>Requisito</t>
   </si>
@@ -160,9 +160,6 @@
     <t>RFD 9.2.1</t>
   </si>
   <si>
-    <t>EsitoDomanda</t>
-  </si>
-  <si>
     <t>MostraDatiD</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>MostraDatiAA</t>
   </si>
   <si>
-    <t>***</t>
-  </si>
-  <si>
     <t>RFOB 22.1</t>
   </si>
   <si>
@@ -244,9 +238,6 @@
     <t>RFOB 9.1</t>
   </si>
   <si>
-    <t>ControlEsitoDom</t>
-  </si>
-  <si>
     <t>ControlMostraDatiD</t>
   </si>
   <si>
@@ -406,9 +397,6 @@
     <t>GestioneTrofeiAA</t>
   </si>
   <si>
-    <t>GestioneRecuperoD</t>
-  </si>
-  <si>
     <t>Da cambiare il nome della classe</t>
   </si>
   <si>
@@ -460,9 +448,6 @@
     <t>Trofei</t>
   </si>
   <si>
-    <t>log?</t>
-  </si>
-  <si>
     <t>Domanda</t>
   </si>
   <si>
@@ -478,13 +463,16 @@
     <t>Altri Requisiti</t>
   </si>
   <si>
-    <t>XXXXXXX</t>
-  </si>
-  <si>
-    <t>Log</t>
-  </si>
-  <si>
     <t>Socket</t>
+  </si>
+  <si>
+    <t>GestioneRecupero</t>
+  </si>
+  <si>
+    <t>AccessLog</t>
+  </si>
+  <si>
+    <t>RVOB 1</t>
   </si>
 </sst>
 </file>
@@ -833,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
@@ -857,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5" customHeight="1">
@@ -871,7 +859,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" customHeight="1">
@@ -881,7 +869,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" customHeight="1">
@@ -891,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" customHeight="1">
@@ -901,7 +889,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1">
@@ -1003,7 +991,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.5" customHeight="1">
@@ -1017,7 +1005,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" customHeight="1">
@@ -1027,7 +1015,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" customHeight="1">
@@ -1107,12 +1095,28 @@
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B27" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" customHeight="1">
+      <c r="C28" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16.5" customHeight="1">
+      <c r="C29" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16.5" customHeight="1">
+      <c r="C30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1122,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C119" sqref="C116:C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -1148,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
@@ -1162,7 +1166,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
@@ -1170,7 +1174,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
@@ -1178,7 +1182,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
@@ -1186,7 +1190,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
@@ -1194,7 +1198,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
@@ -1208,7 +1212,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
@@ -1216,7 +1220,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
@@ -1239,7 +1243,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
@@ -1262,32 +1266,32 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1">
+    <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1">
+    <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="C18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1">
+    <row r="19" spans="1:3" ht="15" customHeight="1">
       <c r="C19" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1">
+    <row r="20" spans="1:3" ht="15" customHeight="1">
       <c r="C20" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1">
+    <row r="21" spans="1:3" ht="15" customHeight="1">
       <c r="C21" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1">
+    <row r="22" spans="1:3" ht="15" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1298,12 +1302,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1">
+    <row r="23" spans="1:3" ht="15" customHeight="1">
       <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1">
+    <row r="24" spans="1:3" ht="15" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1314,37 +1318,37 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1">
+    <row r="25" spans="1:3" ht="15" customHeight="1">
       <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1">
+    <row r="26" spans="1:3" ht="15" customHeight="1">
       <c r="C26" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1">
+    <row r="27" spans="1:3" ht="15" customHeight="1">
       <c r="C27" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1">
+    <row r="28" spans="1:3" ht="15" customHeight="1">
       <c r="C28" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1">
+    <row r="29" spans="1:3" ht="15" customHeight="1">
       <c r="C29" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1">
+    <row r="30" spans="1:3" ht="15" customHeight="1">
       <c r="C30" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1">
+    <row r="31" spans="1:3" ht="15" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -1352,58 +1356,49 @@
         <v>47</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" customHeight="1">
+      <c r="C32" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" customHeight="1">
+      <c r="A33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" customHeight="1">
+      <c r="C34" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" customHeight="1">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1">
-      <c r="A32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1">
-      <c r="C33" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1">
       <c r="C35" s="3" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1">
-      <c r="A36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="C36" s="3" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" customHeight="1">
       <c r="C37" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1">
@@ -1413,559 +1408,540 @@
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1">
       <c r="C39" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1">
       <c r="C40" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" customHeight="1">
+      <c r="A41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1">
-      <c r="C41" s="3" t="s">
+    <row r="42" spans="1:3" ht="15" customHeight="1">
+      <c r="C42" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:3" ht="15" customHeight="1">
+      <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1">
       <c r="C43" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15" customHeight="1">
-      <c r="A44" s="1" t="s">
+      <c r="C44" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" customHeight="1">
+      <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" customHeight="1">
+      <c r="C46" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" customHeight="1">
+      <c r="A47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" customHeight="1">
+      <c r="C48" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15" customHeight="1">
-      <c r="C45" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15" customHeight="1">
-      <c r="A46" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1">
-      <c r="C47" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1">
-      <c r="A48" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" customHeight="1">
       <c r="C49" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1">
+      <c r="A50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C50" s="3" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1">
-      <c r="A51" s="1" t="s">
+      <c r="C51" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15" customHeight="1">
+      <c r="A52" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1">
+      <c r="B52" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="C52" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" customHeight="1">
+      <c r="C53" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15" customHeight="1">
+      <c r="A54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1">
-      <c r="A53" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="1" t="s">
+      <c r="C54" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15" customHeight="1">
+      <c r="C55" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1">
-      <c r="C54" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1">
-      <c r="A55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15" customHeight="1">
       <c r="C56" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15" customHeight="1">
-      <c r="C57" s="3" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="58" spans="1:3" ht="15" customHeight="1">
+      <c r="A58" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="59" spans="1:3" ht="15" customHeight="1">
-      <c r="A59" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C59" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15" customHeight="1">
       <c r="C60" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" customHeight="1">
-      <c r="C61" s="1" t="s">
-        <v>27</v>
+      <c r="A61" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15" customHeight="1">
-      <c r="A62" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C62" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15" customHeight="1">
       <c r="C63" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15" customHeight="1">
       <c r="C64" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15" customHeight="1">
       <c r="C65" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15" customHeight="1">
       <c r="C66" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15" customHeight="1">
-      <c r="C67" s="2" t="s">
-        <v>16</v>
+      <c r="C67" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1">
       <c r="C68" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1">
       <c r="C69" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1">
       <c r="C70" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1">
       <c r="C71" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15" customHeight="1">
       <c r="C72" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15" customHeight="1">
       <c r="C73" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15" customHeight="1">
       <c r="C74" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1">
       <c r="C75" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15" customHeight="1">
-      <c r="C76" s="3" t="s">
-        <v>36</v>
+      <c r="A76" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>4</v>
+        <v>71</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15" customHeight="1">
-      <c r="A78" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C78" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15" customHeight="1">
       <c r="C79" s="3" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15" customHeight="1">
       <c r="C80" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15" customHeight="1">
+      <c r="C81" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15" customHeight="1">
+      <c r="C82" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15" customHeight="1">
+      <c r="C83" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15" customHeight="1">
+      <c r="C84" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15" customHeight="1">
+      <c r="A85" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15" customHeight="1">
+      <c r="C86" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15" customHeight="1">
+      <c r="A87" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1">
-      <c r="C81" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1">
-      <c r="C82" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1">
-      <c r="C83" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1">
-      <c r="C84" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1">
-      <c r="C85" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1">
-      <c r="A86" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B86" s="1" t="s">
+      <c r="C87" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15" customHeight="1">
+      <c r="C88" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15" customHeight="1">
+      <c r="A89" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1">
-      <c r="A87" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B87" s="1" t="s">
+      <c r="C89" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15" customHeight="1">
+      <c r="C90" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15" customHeight="1">
+      <c r="C91" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15" customHeight="1">
+      <c r="C92" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15" customHeight="1">
+      <c r="A93" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C87" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1">
-      <c r="C88" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1">
-      <c r="A89" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B89" s="1" t="s">
+      <c r="C93" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15" customHeight="1">
+      <c r="C94" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15" customHeight="1">
+      <c r="C95" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15" customHeight="1">
+      <c r="C96" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15" customHeight="1">
+      <c r="C97" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15" customHeight="1">
+      <c r="A98" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1">
-      <c r="C90" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1">
-      <c r="A91" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1">
-      <c r="C92" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1">
-      <c r="C93" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1">
-      <c r="C94" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1">
-      <c r="A95" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1">
-      <c r="C96" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="15" customHeight="1">
-      <c r="C97" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="15" customHeight="1">
       <c r="C98" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15" customHeight="1">
       <c r="C99" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15" customHeight="1">
       <c r="C101" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15" customHeight="1">
-      <c r="A102" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="C102" s="3" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15" customHeight="1">
       <c r="C103" s="3" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15" customHeight="1">
+      <c r="A104" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="C104" s="3" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15" customHeight="1">
       <c r="C105" s="3" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15" customHeight="1">
       <c r="A106" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15" customHeight="1">
       <c r="C107" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15" customHeight="1">
       <c r="A108" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15" customHeight="1">
       <c r="C109" s="3" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15" customHeight="1">
-      <c r="A110" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C110" s="3" t="s">
+      <c r="C110" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15" customHeight="1">
+      <c r="A111" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15" customHeight="1">
+      <c r="C112" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15" customHeight="1">
+      <c r="C113" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15" customHeight="1">
-      <c r="C111" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="15" customHeight="1">
-      <c r="C112" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="15" customHeight="1">
-      <c r="A113" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="114" spans="1:3" ht="15" customHeight="1">
+      <c r="A114" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C114" s="3" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="15" customHeight="1">
       <c r="C115" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="15" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="15" customHeight="1">
       <c r="C117" s="3" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15" customHeight="1">
-      <c r="A118" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B118" s="1" t="s">
+      <c r="C118" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="15" customHeight="1">
       <c r="C119" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="15" customHeight="1">
-      <c r="C120" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="15" customHeight="1">
-      <c r="C121" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2002,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
@@ -2010,13 +1986,13 @@
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
@@ -2024,7 +2000,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
@@ -2032,7 +2008,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
@@ -2040,7 +2016,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
@@ -2048,7 +2024,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
@@ -2056,13 +2032,13 @@
         <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
@@ -2095,7 +2071,7 @@
         <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
@@ -2103,7 +2079,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1">
       <c r="C14" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
@@ -2116,7 +2092,7 @@
         <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>13</v>
@@ -2124,7 +2100,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="C17" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
@@ -2132,7 +2108,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>15</v>
@@ -2140,7 +2116,7 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="C19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
@@ -2148,7 +2124,7 @@
         <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>40</v>
@@ -2189,7 +2165,7 @@
         <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>6</v>
@@ -2207,33 +2183,33 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="C32" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
       <c r="C33" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
       <c r="C34" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>9</v>
@@ -2254,23 +2230,23 @@
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1">
       <c r="C40" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1">
       <c r="C41" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1">
@@ -2280,22 +2256,22 @@
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1">
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1">
       <c r="C44" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1">
       <c r="C45" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1">
       <c r="C46" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1">
@@ -2305,15 +2281,15 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1">
       <c r="C48" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>40</v>
@@ -2351,46 +2327,46 @@
     </row>
     <row r="56" spans="1:3" ht="15.75" customHeight="1">
       <c r="C56" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" customHeight="1">
       <c r="C57" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" customHeight="1">
       <c r="C58" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" customHeight="1">
       <c r="C59" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" customHeight="1">
       <c r="C61" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>10</v>
@@ -2409,10 +2385,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -2424,7 +2400,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2435,12 +2411,12 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
@@ -2448,20 +2424,29 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
+      <c r="D2" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1">
+      <c r="D3" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1">
+      <c r="D4" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
@@ -2469,80 +2454,87 @@
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1">
+      <c r="D5" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1">
+      <c r="D6" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1">
+    <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1">
+    <row r="11" spans="1:5" ht="15" customHeight="1">
       <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1">
+    <row r="12" spans="1:5" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1">
+    <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1">
+    <row r="14" spans="1:5" ht="15" customHeight="1">
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1">
+    <row r="16" spans="1:5" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="C17" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
@@ -2565,10 +2557,10 @@
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
@@ -2626,10 +2618,10 @@
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>33</v>
@@ -2637,7 +2629,7 @@
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1">
       <c r="C34" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1">
@@ -2647,20 +2639,20 @@
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1">
       <c r="C36" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" customHeight="1">
       <c r="C37" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>13</v>
@@ -2668,15 +2660,15 @@
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1">
       <c r="C39" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>30</v>
@@ -2684,15 +2676,15 @@
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1">
       <c r="C41" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>14</v>
@@ -2700,17 +2692,17 @@
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1">
       <c r="C43" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15" customHeight="1">
       <c r="C44" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" customHeight="1">
       <c r="C45" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15" customHeight="1">
@@ -2720,33 +2712,33 @@
     </row>
     <row r="47" spans="1:3" ht="15" customHeight="1">
       <c r="C47" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" customHeight="1">
       <c r="C48" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1">
       <c r="C49" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1">
       <c r="C51" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1">
@@ -2756,15 +2748,15 @@
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1">
       <c r="C53" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>13</v>
@@ -2772,15 +2764,15 @@
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1">
       <c r="C55" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>30</v>
@@ -2788,26 +2780,26 @@
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="C57" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1">
       <c r="C59" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1">
@@ -2817,21 +2809,21 @@
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>4</v>
@@ -2849,23 +2841,23 @@
     </row>
     <row r="67" spans="1:3" ht="15" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1">
       <c r="C68" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1">
       <c r="C69" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1">
@@ -2875,22 +2867,22 @@
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1">
       <c r="C71" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15" customHeight="1">
       <c r="C72" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15" customHeight="1">
       <c r="C73" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15" customHeight="1">
       <c r="C74" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1">
@@ -2900,15 +2892,15 @@
     </row>
     <row r="76" spans="1:3" ht="15" customHeight="1">
       <c r="C76" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>40</v>
@@ -2946,226 +2938,224 @@
     </row>
     <row r="84" spans="1:3" ht="15" customHeight="1">
       <c r="C84" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15" customHeight="1">
       <c r="C85" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1">
       <c r="C86" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1">
       <c r="C87" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1">
       <c r="A88" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="C88" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15" customHeight="1">
       <c r="C89" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15" customHeight="1">
       <c r="C91" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15" customHeight="1">
       <c r="C93" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15" customHeight="1">
       <c r="C94" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15" customHeight="1">
       <c r="C95" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15" customHeight="1">
       <c r="C96" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15" customHeight="1">
+      <c r="A97" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="B97" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1">
-      <c r="A98" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B98" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15" customHeight="1">
+      <c r="C98" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15" customHeight="1">
+      <c r="A100" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1">
-      <c r="C99" s="1" t="s">
+    <row r="101" spans="1:3" ht="15" customHeight="1">
+      <c r="C101" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1">
-      <c r="C100" s="1" t="s">
+    <row r="102" spans="1:3" ht="15" customHeight="1">
+      <c r="C102" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1">
-      <c r="A101" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1">
-      <c r="C102" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1">
+    <row r="103" spans="1:3" ht="15" customHeight="1">
+      <c r="A103" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="C103" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15" customHeight="1">
       <c r="C104" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15" customHeight="1">
+      <c r="C105" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15" customHeight="1">
+      <c r="C106" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1">
-      <c r="C105" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1">
-      <c r="C106" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1">
+    <row r="107" spans="1:3" ht="15" customHeight="1">
       <c r="C107" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15" customHeight="1">
       <c r="C108" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15" customHeight="1">
       <c r="C109" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15" customHeight="1">
+      <c r="C110" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15" customHeight="1">
+      <c r="C111" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1">
-      <c r="C110" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1">
-      <c r="A111" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C111" s="3" t="s">
+    <row r="112" spans="1:3" ht="15" customHeight="1">
+      <c r="C112" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15" customHeight="1">
+      <c r="A113" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1">
-      <c r="C112" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1">
-      <c r="C113" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1">
       <c r="C114" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1">
       <c r="C115" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1">
       <c r="C116" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1">
       <c r="C117" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1">
-      <c r="C118" s="1" t="s">
-        <v>139</v>
+      <c r="C118" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1">
       <c r="C119" s="3" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1">
-      <c r="C120" s="3" t="s">
-        <v>62</v>
+      <c r="C120" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1">
@@ -3174,58 +3164,59 @@
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1">
-      <c r="A122" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D122" s="4"/>
+      <c r="C122" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1">
-      <c r="C123" s="1" t="s">
-        <v>67</v>
+      <c r="C123" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1">
       <c r="A124" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D124" s="4"/>
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1">
       <c r="C125" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1">
       <c r="A126" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C126" s="3"/>
-      <c r="D126" s="1" t="s">
-        <v>153</v>
+        <v>142</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1">
-      <c r="C127" s="3"/>
+      <c r="C127" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1">
       <c r="C128" s="3"/>
     </row>
     <row r="129" spans="3:3" ht="15" customHeight="1">
       <c r="C129" s="3"/>
+    </row>
+    <row r="130" spans="3:3" ht="15" customHeight="1">
+      <c r="C130" s="3"/>
+    </row>
+    <row r="131" spans="3:3" ht="15" customHeight="1">
+      <c r="C131" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RQ - ST: cap 10 e piccoli fix al xlsx
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Specifica Tecnica/Tracciamento Classi-requisiti.xlsx
+++ b/RQ/Esterni/Specifica Tecnica/Tracciamento Classi-requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="10515" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="10515" windowHeight="7485" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Desktop" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="150">
   <si>
     <t>Requisito</t>
   </si>
@@ -397,9 +397,6 @@
     <t>GestioneTrofeiAA</t>
   </si>
   <si>
-    <t>Da cambiare il nome della classe</t>
-  </si>
-  <si>
     <t>……..</t>
   </si>
   <si>
@@ -455,9 +452,6 @@
   </si>
   <si>
     <t>Recupero</t>
-  </si>
-  <si>
-    <t>For all in pagine…</t>
   </si>
   <si>
     <t>Altri Requisiti</t>
@@ -821,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
@@ -845,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5" customHeight="1">
@@ -970,7 +964,6 @@
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="16.5" customHeight="1">
       <c r="A15" s="2"/>
@@ -978,41 +971,35 @@
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>91</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="16.5" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>93</v>
@@ -1022,39 +1009,42 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="16.5" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D22" s="2"/>
     </row>
@@ -1062,7 +1052,7 @@
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" s="2"/>
     </row>
@@ -1070,7 +1060,7 @@
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D24" s="2"/>
     </row>
@@ -1078,45 +1068,53 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A26" s="2" t="s">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A27" s="1" t="s">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16.5" customHeight="1">
-      <c r="C28" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" customHeight="1">
       <c r="C29" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16.5" customHeight="1">
+      <c r="C30" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5" customHeight="1">
-      <c r="C30" s="3"/>
+    <row r="31" spans="1:4" ht="16.5" customHeight="1">
+      <c r="C31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1128,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C119" sqref="C116:C119"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D60" sqref="D58:D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -1152,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
@@ -1242,9 +1240,6 @@
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="C13" s="3" t="s">
@@ -1480,12 +1475,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1">
+    <row r="49" spans="1:4" ht="15" customHeight="1">
       <c r="C49" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1">
+    <row r="50" spans="1:4" ht="15" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -1496,12 +1491,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15" customHeight="1">
+    <row r="51" spans="1:4" ht="15" customHeight="1">
       <c r="C51" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1">
+    <row r="52" spans="1:4" ht="15" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>25</v>
       </c>
@@ -1512,12 +1507,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1">
+    <row r="53" spans="1:4" ht="15" customHeight="1">
       <c r="C53" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1">
+    <row r="54" spans="1:4" ht="15" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>25</v>
       </c>
@@ -1528,17 +1523,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1">
+    <row r="55" spans="1:4" ht="15" customHeight="1">
       <c r="C55" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" customHeight="1">
+    <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="C56" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15" customHeight="1">
+    <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
@@ -1548,18 +1543,27 @@
       <c r="C58" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="15" customHeight="1">
+      <c r="D58" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" customHeight="1">
       <c r="C59" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="15" customHeight="1">
+      <c r="D59" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" customHeight="1">
       <c r="C60" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="15" customHeight="1">
+      <c r="D60" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>70</v>
       </c>
@@ -1570,17 +1574,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15" customHeight="1">
+    <row r="62" spans="1:4" ht="15" customHeight="1">
       <c r="C62" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15" customHeight="1">
+    <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="C63" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15" customHeight="1">
+    <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="C64" s="2" t="s">
         <v>15</v>
       </c>
@@ -1954,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
@@ -1978,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
@@ -2098,12 +2102,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="C17" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
@@ -2114,12 +2118,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="C19" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
@@ -2130,37 +2134,37 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="C22" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="C23" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="C24" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="C25" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="C26" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -2171,17 +2175,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
       <c r="C28" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
       <c r="C29" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>106</v>
       </c>
@@ -2191,10 +2195,16 @@
       <c r="C31" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D31" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
       <c r="C32" s="3" t="s">
         <v>85</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
@@ -2233,7 +2243,7 @@
         <v>108</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>54</v>
@@ -2241,12 +2251,12 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1">
       <c r="C40" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1">
       <c r="C41" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1">
@@ -2289,7 +2299,7 @@
         <v>108</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>40</v>
@@ -2327,7 +2337,7 @@
     </row>
     <row r="56" spans="1:3" ht="15.75" customHeight="1">
       <c r="C56" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" customHeight="1">
@@ -2350,7 +2360,7 @@
         <v>108</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>66</v>
@@ -2366,7 +2376,7 @@
         <v>108</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>10</v>
@@ -2385,10 +2395,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:XFD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -2411,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
@@ -2433,7 +2443,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
@@ -2455,7 +2465,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
@@ -2463,7 +2473,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
@@ -2720,12 +2730,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1">
+    <row r="49" spans="1:3" ht="15" customHeight="1">
       <c r="C49" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1">
+    <row r="50" spans="1:3" ht="15" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>112</v>
       </c>
@@ -2736,22 +2746,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1">
+    <row r="51" spans="1:3" ht="15" customHeight="1">
       <c r="C51" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1">
+    <row r="52" spans="1:3" ht="15" customHeight="1">
       <c r="C52" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1">
+    <row r="53" spans="1:3" ht="15" customHeight="1">
       <c r="C53" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1">
+    <row r="54" spans="1:3" ht="15" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>112</v>
       </c>
@@ -2762,12 +2772,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1">
+    <row r="55" spans="1:3" ht="15" customHeight="1">
       <c r="C55" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1">
+    <row r="56" spans="1:3" ht="15" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>112</v>
       </c>
@@ -2778,36 +2788,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1">
+    <row r="57" spans="1:3" ht="15" customHeight="1">
       <c r="C57" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1">
+    <row r="58" spans="1:3" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1">
+    </row>
+    <row r="59" spans="1:3" ht="15" customHeight="1">
       <c r="C59" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1">
+    <row r="60" spans="1:3" ht="15" customHeight="1">
       <c r="C60" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1">
+    <row r="61" spans="1:3" ht="15" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>112</v>
       </c>
@@ -2815,39 +2822,44 @@
         <v>113</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15" customHeight="1">
+      <c r="A63" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1">
-      <c r="A64" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="C63" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15" customHeight="1">
       <c r="C64" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15" customHeight="1">
       <c r="C65" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15" customHeight="1">
+      <c r="A66" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="C66" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15" customHeight="1">
-      <c r="A67" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="C67" s="1" t="s">
-        <v>54</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1">
@@ -2857,214 +2869,214 @@
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1">
       <c r="C69" s="1" t="s">
-        <v>135</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1">
       <c r="C70" s="1" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1">
       <c r="C71" s="1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15" customHeight="1">
       <c r="C72" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15" customHeight="1">
       <c r="C73" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15" customHeight="1">
       <c r="C74" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1">
       <c r="C75" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15" customHeight="1">
-      <c r="C76" s="1" t="s">
-        <v>50</v>
+      <c r="A76" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1">
-      <c r="A77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C77" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15" customHeight="1">
       <c r="C78" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15" customHeight="1">
       <c r="C79" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15" customHeight="1">
       <c r="C80" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15" customHeight="1">
       <c r="C81" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15" customHeight="1">
       <c r="C82" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15" customHeight="1">
-      <c r="C83" s="3" t="s">
-        <v>46</v>
+      <c r="C83" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15" customHeight="1">
-      <c r="C84" s="1" t="s">
-        <v>135</v>
+      <c r="C84" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15" customHeight="1">
       <c r="C85" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1">
       <c r="C86" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1">
-      <c r="C87" s="3" t="s">
-        <v>61</v>
+      <c r="A87" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1">
-      <c r="A88" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15" customHeight="1">
+      <c r="A89" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15" customHeight="1">
-      <c r="C89" s="1" t="s">
+    <row r="90" spans="1:3" ht="15" customHeight="1">
+      <c r="C90" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15" customHeight="1">
-      <c r="A90" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="91" spans="1:3" ht="15" customHeight="1">
-      <c r="C91" s="1" t="s">
-        <v>65</v>
+      <c r="A91" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15" customHeight="1">
-      <c r="A92" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="C92" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15" customHeight="1">
       <c r="C93" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15" customHeight="1">
       <c r="C94" s="3" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15" customHeight="1">
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15" customHeight="1">
+      <c r="A96" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="C96" s="1" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15" customHeight="1">
-      <c r="A97" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="C97" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="15" customHeight="1">
-      <c r="C98" s="1" t="s">
         <v>117</v>
       </c>
     </row>
+    <row r="99" spans="1:3" ht="15" customHeight="1">
+      <c r="A99" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="100" spans="1:3" ht="15" customHeight="1">
-      <c r="A100" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C100" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15" customHeight="1">
       <c r="C101" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15" customHeight="1">
+      <c r="A102" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="C102" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15" customHeight="1">
-      <c r="A103" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="C103" s="1" t="s">
-        <v>54</v>
+        <v>133</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15" customHeight="1">
@@ -3074,137 +3086,135 @@
     </row>
     <row r="105" spans="1:3" ht="15" customHeight="1">
       <c r="C105" s="1" t="s">
-        <v>135</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15" customHeight="1">
       <c r="C106" s="1" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15" customHeight="1">
       <c r="C107" s="1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15" customHeight="1">
       <c r="C108" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15" customHeight="1">
       <c r="C109" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15" customHeight="1">
       <c r="C110" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15" customHeight="1">
       <c r="C111" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15" customHeight="1">
-      <c r="C112" s="1" t="s">
-        <v>50</v>
+      <c r="A112" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1">
-      <c r="A113" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="C113" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1">
       <c r="C114" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1">
       <c r="C115" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1">
       <c r="C116" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1">
       <c r="C117" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1">
       <c r="C118" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1">
-      <c r="C119" s="3" t="s">
-        <v>46</v>
+      <c r="C119" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1">
-      <c r="C120" s="1" t="s">
-        <v>135</v>
+      <c r="C120" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1">
       <c r="C121" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1">
       <c r="C122" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1">
-      <c r="C123" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="A123" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D123" s="4"/>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1">
-      <c r="A124" s="1" t="s">
+      <c r="C124" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="15" customHeight="1">
+      <c r="A125" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B125" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C125" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D124" s="4"/>
-    </row>
-    <row r="125" spans="1:4" ht="15" customHeight="1">
-      <c r="C125" s="1" t="s">
+    </row>
+    <row r="126" spans="1:4" ht="15" customHeight="1">
+      <c r="C126" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" customHeight="1">
-      <c r="A126" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="127" spans="1:4" ht="15" customHeight="1">
-      <c r="C127" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="C127" s="3"/>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1">
       <c r="C128" s="3"/>
@@ -3214,9 +3224,6 @@
     </row>
     <row r="130" spans="3:3" ht="15" customHeight="1">
       <c r="C130" s="3"/>
-    </row>
-    <row r="131" spans="3:3" ht="15" customHeight="1">
-      <c r="C131" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RQ - ST un po di aggiornamenti su cap 10-11 e xlsx
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Specifica Tecnica/Tracciamento Classi-requisiti.xlsx
+++ b/RQ/Esterni/Specifica Tecnica/Tracciamento Classi-requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="10515" windowHeight="7485" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="10515" windowHeight="7485" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Desktop" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="150">
   <si>
     <t>Requisito</t>
   </si>
@@ -457,9 +457,6 @@
     <t>Altri Requisiti</t>
   </si>
   <si>
-    <t>Socket</t>
-  </si>
-  <si>
     <t>GestioneRecupero</t>
   </si>
   <si>
@@ -467,6 +464,9 @@
   </si>
   <si>
     <t>RVOB 1</t>
+  </si>
+  <si>
+    <t>ConnBack</t>
   </si>
 </sst>
 </file>
@@ -818,7 +818,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
@@ -1097,7 +1097,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>84</v>
@@ -1552,7 +1552,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1">
@@ -1956,10 +1956,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
@@ -2016,30 +2016,30 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C5" s="1" t="s">
-        <v>26</v>
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C6" s="1" t="s">
-        <v>27</v>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>86</v>
@@ -2047,48 +2047,54 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1">
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1">
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C11" s="2" t="s">
+      <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+      <c r="C12" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C14" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
       <c r="C15" s="3" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
@@ -2096,15 +2102,15 @@
         <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="C17" s="3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
@@ -2112,281 +2118,225 @@
         <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="C19" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="C21" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="C22" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="C23" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="C24" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="C25" s="3" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="C26" s="3" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C28" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="C29" s="3" t="s">
-        <v>12</v>
+        <v>84</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+      <c r="C30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="C31" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1">
       <c r="C32" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C33" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C34" s="3" t="s">
-        <v>87</v>
+      <c r="A34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C35" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="1" t="s">
+      <c r="C36" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A37" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B37" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="C37" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1">
       <c r="C38" s="1" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A39" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>54</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1">
       <c r="C40" s="1" t="s">
-        <v>133</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1">
       <c r="C41" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1">
       <c r="C42" s="1" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C43" s="1" t="s">
-        <v>48</v>
+      <c r="A43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C45" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C46" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C47" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C48" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C49" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C50" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A51" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C45" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C46" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C47" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C48" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A49" s="1" t="s">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A52" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C50" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C51" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1">
+      <c r="B52" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="C52" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C53" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C54" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C55" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C56" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C57" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C58" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C59" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A60" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C61" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="C61" s="3"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A62" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C63" s="3"/>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C64" s="3"/>
+      <c r="C62" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2397,8 +2347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:XFD63"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -2465,7 +2415,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
@@ -2798,7 +2748,7 @@
         <v>112</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>10</v>
@@ -2999,7 +2949,7 @@
       <c r="A91" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -3031,7 +2981,7 @@
         <v>127</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
RQ-ST tracciamenti manca il front end web
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Specifica Tecnica/Tracciamento Classi-requisiti.xlsx
+++ b/RQ/Esterni/Specifica Tecnica/Tracciamento Classi-requisiti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="10515" windowHeight="7485" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="10515" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="Desktop" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="150">
   <si>
     <t>Requisito</t>
   </si>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
@@ -1105,11 +1105,6 @@
     </row>
     <row r="29" spans="1:4" ht="16.5" customHeight="1">
       <c r="C29" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16.5" customHeight="1">
-      <c r="C30" s="3" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1956,10 +1951,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
@@ -2191,7 +2186,7 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1">
       <c r="C30" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>148</v>
@@ -2199,115 +2194,121 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1">
       <c r="C31" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C32" s="3" t="s">
         <v>87</v>
       </c>
     </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
       <c r="C35" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="C36" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A37" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>54</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1">
       <c r="C38" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1">
       <c r="C39" s="1" t="s">
-        <v>134</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1">
       <c r="C40" s="1" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1">
       <c r="C41" s="1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C42" s="1" t="s">
-        <v>66</v>
+      <c r="A42" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A43" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="C43" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1">
       <c r="C44" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1">
       <c r="C45" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1">
       <c r="C46" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1">
       <c r="C47" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1">
       <c r="C48" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C49" s="3" t="s">
-        <v>46</v>
+      <c r="C49" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A50" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="C50" s="1" t="s">
-        <v>134</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1">
@@ -2315,28 +2316,17 @@
         <v>108</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A52" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B52" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C60" s="3"/>
     </row>
     <row r="61" spans="1:3" ht="15.75" customHeight="1">
       <c r="C61" s="3"/>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C62" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>